<commit_message>
Updated script: added SEM and MDC, fixed histogram, saved Bland-Altman and histogram figures
</commit_message>
<xml_diff>
--- a/Attain_data_2025.xlsx
+++ b/Attain_data_2025.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbznn\PycharmProjects\ATTAIN\ATTAIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299DD4AD-9B22-4D58-A476-41A07D0DA876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AF217C-745B-4687-A1D2-75B4C47F5E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF5F3E16-E75D-744C-BD2D-984622ED6648}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$O$2:$O$45</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$O$2:$O$45</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -458,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F089F3-7079-BF4E-8FCF-1FD5E03854E8}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>